<commit_message>
Change the percentage of overlap (segment)
Initial experiment: 25% overlap
New experiment: 50% and 75%
</commit_message>
<xml_diff>
--- a/digit_small_digit_matrix/Results/Summary_random_order.xlsx
+++ b/digit_small_digit_matrix/Results/Summary_random_order.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\GitHub\Group_Learning\digit_small_digit_matrix\Results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93F3F790-84B2-46DF-A3B0-424C547DA45E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A127BCE5-2034-4E8F-914C-4B0614BF8D9D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{FCA56016-C392-4DF4-98FC-DD49B180471E}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{FCA56016-C392-4DF4-98FC-DD49B180471E}"/>
   </bookViews>
   <sheets>
-    <sheet name="StandardSVM" sheetId="1" r:id="rId1"/>
-    <sheet name="GroupLearning(Majority)" sheetId="2" r:id="rId2"/>
+    <sheet name="25%_overlap" sheetId="4" r:id="rId1"/>
+    <sheet name="50%_overlap" sheetId="3" r:id="rId2"/>
+    <sheet name="75%_overlap" sheetId="5" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -32,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="7">
   <si>
     <t>Repeat</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -51,6 +52,14 @@
   </si>
   <si>
     <t>Test</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SVM</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Group</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -414,16 +423,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E8A280F-78E4-4099-B595-D8800A6B0591}">
-  <dimension ref="A1:E8"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4BB7E229-AB1E-449F-AA19-820606490E6C}">
+  <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>5</v>
+      </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
@@ -459,10 +471,12 @@
         <v>0</v>
       </c>
       <c r="D3">
-        <v>13.8</v>
+        <f>13.8/100</f>
+        <v>0.13800000000000001</v>
       </c>
       <c r="E3">
-        <v>11.6</v>
+        <f>11.6/100</f>
+        <v>0.11599999999999999</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -476,10 +490,12 @@
         <v>0</v>
       </c>
       <c r="D4">
-        <v>3.4</v>
+        <f>3.4/100</f>
+        <v>3.4000000000000002E-2</v>
       </c>
       <c r="E4">
-        <v>22.2</v>
+        <f>22.2/100</f>
+        <v>0.222</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -493,10 +509,12 @@
         <v>0</v>
       </c>
       <c r="D5">
-        <v>2.4</v>
+        <f>2.4/100</f>
+        <v>2.4E-2</v>
       </c>
       <c r="E5">
-        <v>36.200000000000003</v>
+        <f>36.2/100</f>
+        <v>0.36200000000000004</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -510,10 +528,12 @@
         <v>0</v>
       </c>
       <c r="D6">
-        <v>1.8</v>
+        <f>1.8/100</f>
+        <v>1.8000000000000002E-2</v>
       </c>
       <c r="E6">
-        <v>31</v>
+        <f>31/100</f>
+        <v>0.31</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -527,10 +547,12 @@
         <v>0</v>
       </c>
       <c r="D7">
-        <v>15.2</v>
+        <f>15.2/100</f>
+        <v>0.152</v>
       </c>
       <c r="E7">
-        <v>12.4</v>
+        <f>12.4/100</f>
+        <v>0.124</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -544,11 +566,430 @@
       </c>
       <c r="D8">
         <f t="shared" si="0"/>
-        <v>7.3199999999999985</v>
+        <v>7.3200000000000001E-2</v>
       </c>
       <c r="E8">
         <f t="shared" si="0"/>
-        <v>22.68</v>
+        <v>0.22679999999999997</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>6</v>
+      </c>
+      <c r="B10" t="s">
+        <v>1</v>
+      </c>
+      <c r="D10" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>0</v>
+      </c>
+      <c r="B11" t="s">
+        <v>3</v>
+      </c>
+      <c r="C11" t="s">
+        <v>2</v>
+      </c>
+      <c r="D11" t="s">
+        <v>3</v>
+      </c>
+      <c r="E11" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>1</v>
+      </c>
+      <c r="B12">
+        <v>0</v>
+      </c>
+      <c r="C12">
+        <v>0</v>
+      </c>
+      <c r="D12">
+        <f>0.4/100</f>
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="E12">
+        <f>3.6/100</f>
+        <v>3.6000000000000004E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>2</v>
+      </c>
+      <c r="B13">
+        <v>0</v>
+      </c>
+      <c r="C13">
+        <v>0</v>
+      </c>
+      <c r="D13">
+        <f>3.6/100</f>
+        <v>3.6000000000000004E-2</v>
+      </c>
+      <c r="E13">
+        <f>1.4/100</f>
+        <v>1.3999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>3</v>
+      </c>
+      <c r="B14">
+        <v>0</v>
+      </c>
+      <c r="C14">
+        <v>0</v>
+      </c>
+      <c r="D14">
+        <f>2.6/100</f>
+        <v>2.6000000000000002E-2</v>
+      </c>
+      <c r="E14">
+        <f>0.4/100</f>
+        <v>4.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>4</v>
+      </c>
+      <c r="B15">
+        <v>0</v>
+      </c>
+      <c r="C15">
+        <v>0</v>
+      </c>
+      <c r="D15">
+        <f>1.2/100</f>
+        <v>1.2E-2</v>
+      </c>
+      <c r="E15">
+        <f>0.4/100</f>
+        <v>4.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>5</v>
+      </c>
+      <c r="B16">
+        <v>0</v>
+      </c>
+      <c r="C16">
+        <v>0</v>
+      </c>
+      <c r="D16">
+        <f>0.8/100</f>
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="E16">
+        <f>0.8/100</f>
+        <v>8.0000000000000002E-3</v>
+      </c>
+    </row>
+    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B17">
+        <f>AVERAGE(B12:B16)</f>
+        <v>0</v>
+      </c>
+      <c r="C17">
+        <f t="shared" ref="C17:E17" si="1">AVERAGE(C12:C16)</f>
+        <v>0</v>
+      </c>
+      <c r="D17">
+        <f t="shared" si="1"/>
+        <v>1.72E-2</v>
+      </c>
+      <c r="E17">
+        <f t="shared" si="1"/>
+        <v>1.32E-2</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{10218D18-697A-4236-967C-6ED2D6ADD6BD}">
+  <dimension ref="A1:E18"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H14" sqref="H14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>0</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>0.13600000000000001</v>
+      </c>
+      <c r="E3">
+        <v>0.27400000000000002</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <v>0</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <v>0.112</v>
+      </c>
+      <c r="E4">
+        <v>0.39400000000000002</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="B5">
+        <v>0</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <v>0.112</v>
+      </c>
+      <c r="E5">
+        <v>0.34399999999999997</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6">
+        <v>0</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <v>0.24399999999999999</v>
+      </c>
+      <c r="E6">
+        <v>0.21199999999999999</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="B7">
+        <v>0</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <v>0.27200000000000002</v>
+      </c>
+      <c r="E7">
+        <v>0.27800000000000002</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B8">
+        <f>AVERAGE(B3:B7)</f>
+        <v>0</v>
+      </c>
+      <c r="C8">
+        <f t="shared" ref="C8:E8" si="0">AVERAGE(C3:C7)</f>
+        <v>0</v>
+      </c>
+      <c r="D8">
+        <f t="shared" si="0"/>
+        <v>0.17519999999999999</v>
+      </c>
+      <c r="E8">
+        <f t="shared" si="0"/>
+        <v>0.3004</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>6</v>
+      </c>
+      <c r="B11" t="s">
+        <v>1</v>
+      </c>
+      <c r="D11" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>0</v>
+      </c>
+      <c r="B12" t="s">
+        <v>3</v>
+      </c>
+      <c r="C12" t="s">
+        <v>2</v>
+      </c>
+      <c r="D12" t="s">
+        <v>3</v>
+      </c>
+      <c r="E12" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>1</v>
+      </c>
+      <c r="B13">
+        <v>0</v>
+      </c>
+      <c r="C13">
+        <v>0</v>
+      </c>
+      <c r="D13">
+        <v>0.14399999999999999</v>
+      </c>
+      <c r="E13">
+        <v>0.09</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>2</v>
+      </c>
+      <c r="B14">
+        <v>0</v>
+      </c>
+      <c r="C14">
+        <v>0</v>
+      </c>
+      <c r="D14">
+        <v>7.3999999999999996E-2</v>
+      </c>
+      <c r="E14">
+        <v>5.6000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>3</v>
+      </c>
+      <c r="B15">
+        <v>0</v>
+      </c>
+      <c r="C15">
+        <v>0</v>
+      </c>
+      <c r="D15">
+        <v>0.04</v>
+      </c>
+      <c r="E15">
+        <v>0.08</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>4</v>
+      </c>
+      <c r="B16">
+        <v>0</v>
+      </c>
+      <c r="C16">
+        <v>0</v>
+      </c>
+      <c r="D16">
+        <v>0.13400000000000001</v>
+      </c>
+      <c r="E16">
+        <v>7.1999999999999995E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>5</v>
+      </c>
+      <c r="B17">
+        <v>0</v>
+      </c>
+      <c r="C17">
+        <v>0.2</v>
+      </c>
+      <c r="D17">
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="E17">
+        <v>0.21199999999999999</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B18">
+        <f>AVERAGE(B13:B17)</f>
+        <v>0</v>
+      </c>
+      <c r="C18">
+        <f t="shared" ref="C18:E18" si="1">AVERAGE(C13:C17)</f>
+        <v>0.04</v>
+      </c>
+      <c r="D18">
+        <f t="shared" si="1"/>
+        <v>7.9999999999999988E-2</v>
+      </c>
+      <c r="E18">
+        <f t="shared" si="1"/>
+        <v>0.10200000000000001</v>
       </c>
     </row>
   </sheetData>
@@ -558,17 +999,20 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DEF16A3C-C4B5-467E-A938-25032CE6CD8A}">
-  <dimension ref="A1:E8"/>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ADE84A97-21F9-43F3-8A34-7A632EE9498D}">
+  <dimension ref="A1:E18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>5</v>
+      </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
@@ -604,10 +1048,10 @@
         <v>0</v>
       </c>
       <c r="D3">
-        <v>0.4</v>
+        <v>0.14000000000000001</v>
       </c>
       <c r="E3">
-        <v>3.6</v>
+        <v>0.47399999999999998</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -621,10 +1065,10 @@
         <v>0</v>
       </c>
       <c r="D4">
-        <v>3.6</v>
+        <v>0.248</v>
       </c>
       <c r="E4">
-        <v>1.4</v>
+        <v>0.36599999999999999</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -638,10 +1082,10 @@
         <v>0</v>
       </c>
       <c r="D5">
-        <v>2.6</v>
+        <v>0.32600000000000001</v>
       </c>
       <c r="E5">
-        <v>0.4</v>
+        <v>0.29799999999999999</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -655,10 +1099,10 @@
         <v>0</v>
       </c>
       <c r="D6">
-        <v>1.2</v>
+        <v>0.20799999999999999</v>
       </c>
       <c r="E6">
-        <v>0.4</v>
+        <v>0.35</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -672,10 +1116,10 @@
         <v>0</v>
       </c>
       <c r="D7">
-        <v>0.8</v>
+        <v>0.254</v>
       </c>
       <c r="E7">
-        <v>0.8</v>
+        <v>0.34</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -689,11 +1133,136 @@
       </c>
       <c r="D8">
         <f t="shared" si="0"/>
-        <v>1.72</v>
+        <v>0.23519999999999999</v>
       </c>
       <c r="E8">
         <f t="shared" si="0"/>
-        <v>1.32</v>
+        <v>0.36560000000000004</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>6</v>
+      </c>
+      <c r="B11" t="s">
+        <v>1</v>
+      </c>
+      <c r="D11" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>0</v>
+      </c>
+      <c r="B12" t="s">
+        <v>3</v>
+      </c>
+      <c r="C12" t="s">
+        <v>2</v>
+      </c>
+      <c r="D12" t="s">
+        <v>3</v>
+      </c>
+      <c r="E12" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>1</v>
+      </c>
+      <c r="B13">
+        <v>0</v>
+      </c>
+      <c r="C13">
+        <v>0</v>
+      </c>
+      <c r="D13">
+        <v>0.23400000000000001</v>
+      </c>
+      <c r="E13">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>2</v>
+      </c>
+      <c r="B14">
+        <v>0</v>
+      </c>
+      <c r="C14">
+        <v>0</v>
+      </c>
+      <c r="D14">
+        <v>8.4000000000000005E-2</v>
+      </c>
+      <c r="E14">
+        <v>0.41399999999999998</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>3</v>
+      </c>
+      <c r="B15">
+        <v>0</v>
+      </c>
+      <c r="C15">
+        <v>0</v>
+      </c>
+      <c r="D15">
+        <v>9.1999999999999998E-2</v>
+      </c>
+      <c r="E15">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>4</v>
+      </c>
+      <c r="B16">
+        <v>0</v>
+      </c>
+      <c r="C16">
+        <v>0</v>
+      </c>
+      <c r="D16">
+        <v>0.40600000000000003</v>
+      </c>
+      <c r="E16">
+        <v>0.29799999999999999</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>5</v>
+      </c>
+      <c r="D17">
+        <v>0.28399999999999997</v>
+      </c>
+      <c r="E17">
+        <v>0.25600000000000001</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B18">
+        <f>AVERAGE(B13:B17)</f>
+        <v>0</v>
+      </c>
+      <c r="C18">
+        <f t="shared" ref="C18:E18" si="1">AVERAGE(C13:C17)</f>
+        <v>0</v>
+      </c>
+      <c r="D18">
+        <f t="shared" si="1"/>
+        <v>0.22000000000000003</v>
+      </c>
+      <c r="E18">
+        <f t="shared" si="1"/>
+        <v>0.3236</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
application of genetic data
</commit_message>
<xml_diff>
--- a/digit_small_digit_matrix/Results/Summary_random_order.xlsx
+++ b/digit_small_digit_matrix/Results/Summary_random_order.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\GitHub\Group_Learning\digit_small_digit_matrix\Results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A127BCE5-2034-4E8F-914C-4B0614BF8D9D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1E116FD-CBBC-4D7E-A906-FB41982487F2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{FCA56016-C392-4DF4-98FC-DD49B180471E}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="3" xr2:uid="{FCA56016-C392-4DF4-98FC-DD49B180471E}"/>
   </bookViews>
   <sheets>
     <sheet name="25%_overlap" sheetId="4" r:id="rId1"/>
     <sheet name="50%_overlap" sheetId="3" r:id="rId2"/>
     <sheet name="75%_overlap" sheetId="5" r:id="rId3"/>
+    <sheet name="工作表1" sheetId="6" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="8">
   <si>
     <t>Repeat</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -60,6 +61,10 @@
   </si>
   <si>
     <t>Group</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>overlap</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -125,6 +130,1175 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="zh-TW"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>SVM_FN</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>工作表1!$A$8:$A$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>75</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>工作表1!$B$8:$B$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>7.3200000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.17519999999999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.23519999999999999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-5780-48B4-95F8-EE927C51F7ED}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>SVM_FP</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>工作表1!$A$8:$A$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>75</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>工作表1!$C$8:$C$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>0.22679999999999997</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.3004</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.36560000000000004</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-5780-48B4-95F8-EE927C51F7ED}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>Group_FN</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>工作表1!$A$8:$A$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>75</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>工作表1!$F$8:$F$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>1.72E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7.9999999999999988E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.22000000000000003</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-5780-48B4-95F8-EE927C51F7ED}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:v>Group_FP</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent4"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>工作表1!$A$8:$A$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>75</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>工作表1!$G$8:$G$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>1.32E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.10200000000000001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.3236</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-5780-48B4-95F8-EE927C51F7ED}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="409867792"/>
+        <c:axId val="409858280"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="409867792"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" altLang="zh-TW"/>
+                  <a:t>Overlap(%)</a:t>
+                </a:r>
+                <a:endParaRPr lang="zh-TW" altLang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="zh-TW"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="zh-TW"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="409858280"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="409858280"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="zh-TW"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="409867792"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="zh-TW"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="zh-TW"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>400783</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>140677</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>169253</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>159727</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="圖表 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EC009792-F4FF-4AAC-8D9D-08E3EC316ED6}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -427,7 +1601,7 @@
   <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+      <selection activeCell="B17" sqref="B17:C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
@@ -725,7 +1899,7 @@
   <dimension ref="A1:E18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+      <selection activeCell="D18" sqref="D18:E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
@@ -1003,8 +2177,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ADE84A97-21F9-43F3-8A34-7A632EE9498D}">
   <dimension ref="A1:E18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D18" sqref="D18:E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
@@ -1240,6 +2414,12 @@
       <c r="A17">
         <v>5</v>
       </c>
+      <c r="B17">
+        <v>0</v>
+      </c>
+      <c r="C17">
+        <v>0</v>
+      </c>
       <c r="D17">
         <v>0.28399999999999997</v>
       </c>
@@ -1269,4 +2449,160 @@
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D880A496-5EE5-4F3F-A604-B9156A2321DB}">
+  <dimension ref="A5:I10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10:G10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>5</v>
+      </c>
+      <c r="F5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>4</v>
+      </c>
+      <c r="D6" t="s">
+        <v>1</v>
+      </c>
+      <c r="F6" t="s">
+        <v>4</v>
+      </c>
+      <c r="H6" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" t="s">
+        <v>3</v>
+      </c>
+      <c r="C7" t="s">
+        <v>2</v>
+      </c>
+      <c r="D7" t="s">
+        <v>3</v>
+      </c>
+      <c r="E7" t="s">
+        <v>2</v>
+      </c>
+      <c r="F7" t="s">
+        <v>3</v>
+      </c>
+      <c r="G7" t="s">
+        <v>2</v>
+      </c>
+      <c r="H7" t="s">
+        <v>3</v>
+      </c>
+      <c r="I7" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>25</v>
+      </c>
+      <c r="B8">
+        <v>7.3200000000000001E-2</v>
+      </c>
+      <c r="C8">
+        <v>0.22679999999999997</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+      <c r="E8">
+        <v>0</v>
+      </c>
+      <c r="F8">
+        <v>1.72E-2</v>
+      </c>
+      <c r="G8">
+        <v>1.32E-2</v>
+      </c>
+      <c r="H8">
+        <v>0</v>
+      </c>
+      <c r="I8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>50</v>
+      </c>
+      <c r="B9">
+        <v>0.17519999999999999</v>
+      </c>
+      <c r="C9">
+        <v>0.3004</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+      <c r="E9">
+        <v>0</v>
+      </c>
+      <c r="F9">
+        <v>7.9999999999999988E-2</v>
+      </c>
+      <c r="G9">
+        <v>0.10200000000000001</v>
+      </c>
+      <c r="H9">
+        <v>0</v>
+      </c>
+      <c r="I9">
+        <v>0.04</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>75</v>
+      </c>
+      <c r="B10">
+        <v>0.23519999999999999</v>
+      </c>
+      <c r="C10">
+        <v>0.36560000000000004</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+      <c r="E10">
+        <v>0</v>
+      </c>
+      <c r="F10">
+        <v>0.22000000000000003</v>
+      </c>
+      <c r="G10">
+        <v>0.3236</v>
+      </c>
+      <c r="H10">
+        <v>0</v>
+      </c>
+      <c r="I10">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>